<commit_message>
Modificato Report-Checklist.xls per RIS
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111APINFORMATICASRLXX/APINFORMATICA/ENERGYOMEGAPLUS-RIS/3.0.0000/report-checklist.xlsx
+++ b/GATEWAY/A1#111APINFORMATICASRLXX/APINFORMATICA/ENERGYOMEGAPLUS-RIS/3.0.0000/report-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Myr\Omega\Fse2\Accreditamento\5-Pdf e Xml da Inviare\COPIA ENERGYOMEGAPLUS-RIS\3.0.0000\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Myr\Omega\Fse2\Accreditamento\5-Pdf e Xml da Inviare\3-Preparati da Ugo\NuovaCartella\it-fse-accreditamento\GATEWAY\A1#111APINFORMATICASRLXX\APINFORMATICA\ENERGYOMEGAPLUS-RIS\3.0.0000\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F60C42-6964-4FD2-9651-5F799C25CDE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2AFC98E1-F0D6-4B9A-ADF0-FDD2ACB15291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10005" yWindow="0" windowWidth="18795" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -253,10 +253,6 @@
     <t xml:space="preserve">
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>ALERT: Identificativo del documento non presente.
-L’identificativo del documento viene scelto, all’interno della maschera di inserimento, tra un elenco di valori preinseriti. Nell’ipotetico caso in cui l’identificativo non sia scelto, l’operatore di accettazione potrà provvedere alla correzione</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT12_KO</t>
@@ -732,16 +728,33 @@
   <si>
     <t>[ERRORE-40| L'elemento ClinicalDocument/documentationOf/serviceEvent deve contenere l'elemento code e DEVE valorizzare il suo attributo code con uno dei seguenti valori: 'PROG'|'DIR'|'RAD_PROG|'RAD_DIR' ],[W005 | Sezione Esame Eseguito: l'entry/act/code può essere valorizzato secondo i sistemi di codifica\n\t\t\tLOINC @codeSystem='2.16.840.1.113883.6.1'\n\t\t\tICD-9-CM @codeSystem='2.16.840.1.113883.6.103']</t>
   </si>
+  <si>
+    <t>ATTENZIONE: Tipologia di Accesso mancante.
+All'utente viene mostrata una message box riportante il seguente messaggio:
+Non è stata specificata la Tipologia di Accesso.
+Scegliere da menù a tendina una delle seguenti voci:
+‘Accesso Programmato’
+ ’Accesso Diretto’,
+’Accesso Programmato Radiologia’
+ ‘Accesso Diretto Radiologia’</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
@@ -805,6 +818,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -832,7 +851,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1151,23 +1170,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1196,199 +1230,267 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="3" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="3" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="9" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
     <cellStyle name="Normale 2" xfId="1" xr:uid="{4CEF7679-60E4-42E7-9AD0-71C0DEBC44BD}"/>
+    <cellStyle name="Normale 3" xfId="2" xr:uid="{BCE2C5C8-87D9-407E-B70B-8A5CB5AAECCB}"/>
+    <cellStyle name="Normale 4" xfId="3" xr:uid="{E0301326-3BA3-4CEF-9AFC-4985015D1601}"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E2F3"/>
+          <bgColor rgb="FFD9E2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E2F3"/>
+          <bgColor rgb="FFD9E2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E2F3"/>
+          <bgColor rgb="FFD9E2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E2F3"/>
+          <bgColor rgb="FFD9E2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="2">
+    <tableStyle name="Sheet1-style" pivot="0" count="3" xr9:uid="{88A27C37-8D75-4317-93A7-562BB8626A75}">
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="firstRowStripe" dxfId="4"/>
+      <tableStyleElement type="secondRowStripe" dxfId="3"/>
+    </tableStyle>
+    <tableStyle name="Sheet1-style 2" pivot="0" count="3" xr9:uid="{D5FC3BE3-1000-498D-B01B-4DA91CF2E7CF}">
+      <tableStyleElement type="headerRow" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="secondRowStripe" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -2557,28 +2659,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T880"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="O31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.85546875" style="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" style="31" customWidth="1"/>
     <col min="4" max="4" width="41.5703125" style="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="67.42578125" style="31" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" style="67" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.5703125" style="31" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="67" customWidth="1"/>
     <col min="7" max="7" width="15" style="68" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" style="67" customWidth="1"/>
-    <col min="9" max="9" width="74.85546875" style="67" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="72.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.42578125" style="31" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="41.140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="255.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="38.42578125" style="31" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="157.5703125" style="31" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21" style="67" customWidth="1"/>
+    <col min="10" max="10" width="13" style="31" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" style="31" customWidth="1"/>
+    <col min="12" max="12" width="6.42578125" style="31" customWidth="1"/>
+    <col min="13" max="13" width="11" style="31" customWidth="1"/>
+    <col min="14" max="14" width="64.7109375" style="31" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" style="31" customWidth="1"/>
+    <col min="16" max="16" width="91.7109375" style="31" customWidth="1"/>
     <col min="17" max="17" width="7.85546875" style="31" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="28.5703125" style="31" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="7.42578125" style="31" bestFit="1" customWidth="1"/>
@@ -2609,14 +2711,14 @@
       <c r="T1" s="36"/>
     </row>
     <row r="2" spans="1:20" ht="18.75">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="71"/>
-      <c r="C2" s="72" t="s">
-        <v>117</v>
-      </c>
-      <c r="D2" s="73"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="86" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="87"/>
       <c r="E2" s="40"/>
       <c r="F2" s="34"/>
       <c r="G2" s="35"/>
@@ -2635,14 +2737,14 @@
       <c r="T2" s="36"/>
     </row>
     <row r="3" spans="1:20" ht="15.75">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="76" t="s">
-        <v>120</v>
-      </c>
-      <c r="D3" s="77"/>
+      <c r="B3" s="89"/>
+      <c r="C3" s="90" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="91"/>
       <c r="E3" s="40"/>
       <c r="F3" s="34"/>
       <c r="G3" s="35"/>
@@ -2661,12 +2763,12 @@
       <c r="T3" s="36"/>
     </row>
     <row r="4" spans="1:20" ht="15.75">
-      <c r="A4" s="75"/>
-      <c r="B4" s="75"/>
-      <c r="C4" s="76" t="s">
-        <v>118</v>
-      </c>
-      <c r="D4" s="77"/>
+      <c r="A4" s="89"/>
+      <c r="B4" s="89"/>
+      <c r="C4" s="90" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="91"/>
       <c r="E4" s="41"/>
       <c r="F4" s="34"/>
       <c r="G4" s="35"/>
@@ -2685,12 +2787,12 @@
       <c r="T4" s="36"/>
     </row>
     <row r="5" spans="1:20" ht="15.75">
-      <c r="A5" s="75"/>
-      <c r="B5" s="75"/>
-      <c r="C5" s="76" t="s">
-        <v>119</v>
-      </c>
-      <c r="D5" s="77"/>
+      <c r="A5" s="89"/>
+      <c r="B5" s="89"/>
+      <c r="C5" s="90" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="91"/>
       <c r="E5" s="40"/>
       <c r="F5" s="34"/>
       <c r="G5" s="35"/>
@@ -2709,8 +2811,8 @@
       <c r="T5" s="36"/>
     </row>
     <row r="6" spans="1:20">
-      <c r="A6" s="69"/>
-      <c r="B6" s="69"/>
+      <c r="A6" s="83"/>
+      <c r="B6" s="83"/>
       <c r="C6" s="42"/>
       <c r="D6" s="43"/>
       <c r="E6" s="33"/>
@@ -2774,7 +2876,7 @@
       <c r="S8" s="51"/>
       <c r="T8" s="48"/>
     </row>
-    <row r="9" spans="1:20" ht="37.5">
+    <row r="9" spans="1:20" ht="131.25">
       <c r="A9" s="52" t="s">
         <v>2</v>
       </c>
@@ -2836,7 +2938,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="105">
+    <row r="10" spans="1:20" ht="409.5">
       <c r="A10" s="21">
         <v>11</v>
       </c>
@@ -2856,13 +2958,13 @@
         <v>45211</v>
       </c>
       <c r="G10" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="H10" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="H10" s="26" t="s">
+      <c r="I10" s="26" t="s">
         <v>133</v>
-      </c>
-      <c r="I10" s="26" t="s">
-        <v>134</v>
       </c>
       <c r="J10" s="53" t="s">
         <v>26</v>
@@ -2880,7 +2982,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="105">
+    <row r="11" spans="1:20" ht="409.5">
       <c r="A11" s="21">
         <v>12</v>
       </c>
@@ -2900,13 +3002,13 @@
         <v>45211</v>
       </c>
       <c r="G11" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="H11" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="H11" s="26" t="s">
+      <c r="I11" s="26" t="s">
         <v>136</v>
-      </c>
-      <c r="I11" s="26" t="s">
-        <v>137</v>
       </c>
       <c r="J11" s="53" t="s">
         <v>26</v>
@@ -2923,7 +3025,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="105">
+    <row r="12" spans="1:20" ht="409.5">
       <c r="A12" s="21">
         <v>13</v>
       </c>
@@ -2943,13 +3045,13 @@
         <v>45211</v>
       </c>
       <c r="G12" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="H12" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="H12" s="25" t="s">
+      <c r="I12" s="55" t="s">
         <v>139</v>
-      </c>
-      <c r="I12" s="55" t="s">
-        <v>140</v>
       </c>
       <c r="J12" s="53" t="s">
         <v>26</v>
@@ -2967,7 +3069,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="105">
+    <row r="13" spans="1:20" ht="409.5">
       <c r="A13" s="21">
         <v>14</v>
       </c>
@@ -2987,13 +3089,13 @@
         <v>45211</v>
       </c>
       <c r="G13" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="H13" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="H13" s="26" t="s">
+      <c r="I13" s="26" t="s">
         <v>142</v>
-      </c>
-      <c r="I13" s="26" t="s">
-        <v>143</v>
       </c>
       <c r="J13" s="53" t="s">
         <v>26</v>
@@ -3011,7 +3113,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="105">
+    <row r="14" spans="1:20" ht="409.5">
       <c r="A14" s="21">
         <v>31</v>
       </c>
@@ -3025,7 +3127,7 @@
         <v>34</v>
       </c>
       <c r="E14" s="56" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F14" s="24"/>
       <c r="G14" s="25"/>
@@ -3049,7 +3151,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="120">
+    <row r="15" spans="1:20" ht="409.5">
       <c r="A15" s="21">
         <v>39</v>
       </c>
@@ -3063,19 +3165,19 @@
         <v>38</v>
       </c>
       <c r="E15" s="56" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F15" s="24">
         <v>45211</v>
       </c>
       <c r="G15" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="H15" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="H15" s="25" t="s">
+      <c r="I15" s="25" t="s">
         <v>145</v>
-      </c>
-      <c r="I15" s="25" t="s">
-        <v>146</v>
       </c>
       <c r="J15" s="53" t="s">
         <v>26</v>
@@ -3103,7 +3205,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="45">
+    <row r="16" spans="1:20" ht="195">
       <c r="A16" s="21">
         <v>47</v>
       </c>
@@ -3141,7 +3243,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="105">
+    <row r="17" spans="1:20" ht="409.5">
       <c r="A17" s="21">
         <v>75</v>
       </c>
@@ -3179,7 +3281,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="90">
+    <row r="18" spans="1:20" ht="409.5">
       <c r="A18" s="21">
         <v>76</v>
       </c>
@@ -3217,7 +3319,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="75">
+    <row r="19" spans="1:20" ht="409.5">
       <c r="A19" s="21">
         <v>77</v>
       </c>
@@ -3237,13 +3339,13 @@
         <v>45211</v>
       </c>
       <c r="G19" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="H19" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="H19" s="26" t="s">
+      <c r="I19" s="26" t="s">
         <v>148</v>
-      </c>
-      <c r="I19" s="26" t="s">
-        <v>149</v>
       </c>
       <c r="J19" s="53" t="s">
         <v>26</v>
@@ -3256,7 +3358,7 @@
         <v>35</v>
       </c>
       <c r="N19" s="28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O19" s="26" t="s">
         <v>26</v>
@@ -3271,7 +3373,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="75">
+    <row r="20" spans="1:20" ht="409.5">
       <c r="A20" s="21">
         <v>78</v>
       </c>
@@ -3291,13 +3393,13 @@
         <v>45211</v>
       </c>
       <c r="G20" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="H20" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="H20" s="26" t="s">
+      <c r="I20" s="26" t="s">
         <v>151</v>
-      </c>
-      <c r="I20" s="26" t="s">
-        <v>152</v>
       </c>
       <c r="J20" s="53" t="s">
         <v>26</v>
@@ -3310,7 +3412,7 @@
         <v>26</v>
       </c>
       <c r="N20" s="28" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O20" s="26" t="s">
         <v>35</v>
@@ -3325,7 +3427,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="90">
+    <row r="21" spans="1:20" ht="409.5">
       <c r="A21" s="21">
         <v>79</v>
       </c>
@@ -3363,7 +3465,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="90">
+    <row r="22" spans="1:20" ht="409.5">
       <c r="A22" s="21">
         <v>80</v>
       </c>
@@ -3401,61 +3503,61 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:20" s="90" customFormat="1" ht="180">
-      <c r="A23" s="78">
+    <row r="23" spans="1:20" s="81" customFormat="1" ht="409.5">
+      <c r="A23" s="69">
         <v>81</v>
       </c>
-      <c r="B23" s="79" t="s">
+      <c r="B23" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="79" t="s">
+      <c r="C23" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="79" t="s">
+      <c r="D23" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="E23" s="80" t="s">
+      <c r="E23" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="F23" s="81">
+      <c r="F23" s="72">
         <v>45211</v>
       </c>
-      <c r="G23" s="82" t="s">
+      <c r="G23" s="73" t="s">
+        <v>152</v>
+      </c>
+      <c r="H23" s="74" t="s">
         <v>153</v>
       </c>
-      <c r="H23" s="83" t="s">
+      <c r="I23" s="74" t="s">
         <v>154</v>
       </c>
-      <c r="I23" s="83" t="s">
-        <v>155</v>
-      </c>
-      <c r="J23" s="84" t="s">
+      <c r="J23" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="K23" s="85"/>
-      <c r="L23" s="83" t="s">
+      <c r="K23" s="76"/>
+      <c r="L23" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="M23" s="83" t="s">
+      <c r="M23" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="N23" s="86" t="s">
-        <v>123</v>
-      </c>
-      <c r="O23" s="83" t="s">
+      <c r="N23" s="77" t="s">
+        <v>122</v>
+      </c>
+      <c r="O23" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="P23" s="87" t="s">
-        <v>182</v>
-      </c>
-      <c r="Q23" s="88"/>
-      <c r="R23" s="83"/>
-      <c r="S23" s="89"/>
-      <c r="T23" s="83" t="s">
+      <c r="P23" s="78" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q23" s="79"/>
+      <c r="R23" s="74"/>
+      <c r="S23" s="80"/>
+      <c r="T23" s="74" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="90">
+    <row r="24" spans="1:20" ht="409.5">
       <c r="A24" s="21">
         <v>82</v>
       </c>
@@ -3466,10 +3568,10 @@
         <v>23</v>
       </c>
       <c r="D24" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="23" t="s">
         <v>63</v>
-      </c>
-      <c r="E24" s="23" t="s">
-        <v>64</v>
       </c>
       <c r="F24" s="24"/>
       <c r="G24" s="25"/>
@@ -3479,7 +3581,7 @@
         <v>35</v>
       </c>
       <c r="K24" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L24" s="29"/>
       <c r="M24" s="29"/>
@@ -3493,7 +3595,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="75">
+    <row r="25" spans="1:20" ht="409.5">
       <c r="A25" s="21">
         <v>83</v>
       </c>
@@ -3504,10 +3606,10 @@
         <v>23</v>
       </c>
       <c r="D25" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" s="23" t="s">
         <v>66</v>
-      </c>
-      <c r="E25" s="23" t="s">
-        <v>67</v>
       </c>
       <c r="F25" s="24"/>
       <c r="G25" s="25"/>
@@ -3531,7 +3633,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="75">
+    <row r="26" spans="1:20" ht="409.5">
       <c r="A26" s="21">
         <v>84</v>
       </c>
@@ -3542,22 +3644,22 @@
         <v>23</v>
       </c>
       <c r="D26" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26" s="23" t="s">
         <v>68</v>
-      </c>
-      <c r="E26" s="23" t="s">
-        <v>69</v>
       </c>
       <c r="F26" s="24">
         <v>45211</v>
       </c>
       <c r="G26" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="H26" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="H26" s="26" t="s">
+      <c r="I26" s="26" t="s">
         <v>157</v>
-      </c>
-      <c r="I26" s="26" t="s">
-        <v>158</v>
       </c>
       <c r="J26" s="53" t="s">
         <v>26</v>
@@ -3570,13 +3672,13 @@
         <v>26</v>
       </c>
       <c r="N26" s="28" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="O26" s="26" t="s">
         <v>35</v>
       </c>
       <c r="P26" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q26" s="29"/>
       <c r="R26" s="26"/>
@@ -3585,7 +3687,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="90">
+    <row r="27" spans="1:20" ht="409.5">
       <c r="A27" s="21">
         <v>85</v>
       </c>
@@ -3596,10 +3698,10 @@
         <v>23</v>
       </c>
       <c r="D27" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" s="23" t="s">
         <v>71</v>
-      </c>
-      <c r="E27" s="23" t="s">
-        <v>72</v>
       </c>
       <c r="F27" s="24"/>
       <c r="G27" s="25"/>
@@ -3609,7 +3711,7 @@
         <v>35</v>
       </c>
       <c r="K27" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L27" s="29"/>
       <c r="M27" s="29"/>
@@ -3623,7 +3725,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="90">
+    <row r="28" spans="1:20" ht="409.5">
       <c r="A28" s="21">
         <v>86</v>
       </c>
@@ -3634,22 +3736,22 @@
         <v>23</v>
       </c>
       <c r="D28" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="23" t="s">
         <v>74</v>
-      </c>
-      <c r="E28" s="23" t="s">
-        <v>75</v>
       </c>
       <c r="F28" s="24">
         <v>45211</v>
       </c>
       <c r="G28" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="H28" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="H28" s="26" t="s">
+      <c r="I28" s="26" t="s">
         <v>160</v>
-      </c>
-      <c r="I28" s="26" t="s">
-        <v>161</v>
       </c>
       <c r="J28" s="53" t="s">
         <v>26</v>
@@ -3662,13 +3764,13 @@
         <v>26</v>
       </c>
       <c r="N28" s="28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="O28" s="26" t="s">
         <v>35</v>
       </c>
       <c r="P28" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q28" s="29"/>
       <c r="R28" s="26"/>
@@ -3677,7 +3779,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="180">
+    <row r="29" spans="1:20" ht="409.5">
       <c r="A29" s="21">
         <v>87</v>
       </c>
@@ -3688,22 +3790,22 @@
         <v>23</v>
       </c>
       <c r="D29" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="E29" s="23" t="s">
         <v>77</v>
-      </c>
-      <c r="E29" s="23" t="s">
-        <v>78</v>
       </c>
       <c r="F29" s="24">
         <v>45211</v>
       </c>
       <c r="G29" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="H29" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="H29" s="26" t="s">
+      <c r="I29" s="26" t="s">
         <v>163</v>
-      </c>
-      <c r="I29" s="26" t="s">
-        <v>164</v>
       </c>
       <c r="J29" s="53" t="s">
         <v>26</v>
@@ -3716,13 +3818,13 @@
         <v>26</v>
       </c>
       <c r="N29" s="28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O29" s="26" t="s">
         <v>35</v>
       </c>
       <c r="P29" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q29" s="29"/>
       <c r="R29" s="26"/>
@@ -3731,7 +3833,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="90">
+    <row r="30" spans="1:20" ht="409.5">
       <c r="A30" s="21">
         <v>88</v>
       </c>
@@ -3742,22 +3844,22 @@
         <v>23</v>
       </c>
       <c r="D30" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="23" t="s">
         <v>80</v>
-      </c>
-      <c r="E30" s="23" t="s">
-        <v>81</v>
       </c>
       <c r="F30" s="24">
         <v>45211</v>
       </c>
       <c r="G30" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="H30" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="H30" s="26" t="s">
+      <c r="I30" s="26" t="s">
         <v>166</v>
-      </c>
-      <c r="I30" s="26" t="s">
-        <v>167</v>
       </c>
       <c r="J30" s="26" t="s">
         <v>26</v>
@@ -3770,13 +3872,13 @@
         <v>26</v>
       </c>
       <c r="N30" s="28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="O30" s="26" t="s">
         <v>35</v>
       </c>
       <c r="P30" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q30" s="29"/>
       <c r="R30" s="26"/>
@@ -3785,7 +3887,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="75">
+    <row r="31" spans="1:20" ht="409.5">
       <c r="A31" s="21">
         <v>89</v>
       </c>
@@ -3796,22 +3898,22 @@
         <v>23</v>
       </c>
       <c r="D31" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="E31" s="23" t="s">
         <v>83</v>
-      </c>
-      <c r="E31" s="23" t="s">
-        <v>84</v>
       </c>
       <c r="F31" s="24">
         <v>45211</v>
       </c>
       <c r="G31" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="H31" s="26" t="s">
         <v>168</v>
       </c>
-      <c r="H31" s="26" t="s">
+      <c r="I31" s="26" t="s">
         <v>169</v>
-      </c>
-      <c r="I31" s="26" t="s">
-        <v>170</v>
       </c>
       <c r="J31" s="26" t="s">
         <v>26</v>
@@ -3824,13 +3926,13 @@
         <v>26</v>
       </c>
       <c r="N31" s="28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O31" s="26" t="s">
         <v>35</v>
       </c>
       <c r="P31" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q31" s="29"/>
       <c r="R31" s="26"/>
@@ -3839,7 +3941,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="75">
+    <row r="32" spans="1:20" ht="409.5">
       <c r="A32" s="21">
         <v>90</v>
       </c>
@@ -3850,22 +3952,22 @@
         <v>23</v>
       </c>
       <c r="D32" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="E32" s="23" t="s">
         <v>86</v>
-      </c>
-      <c r="E32" s="23" t="s">
-        <v>87</v>
       </c>
       <c r="F32" s="24">
         <v>45211</v>
       </c>
       <c r="G32" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="H32" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="H32" s="25" t="s">
+      <c r="I32" s="55" t="s">
         <v>172</v>
-      </c>
-      <c r="I32" s="55" t="s">
-        <v>173</v>
       </c>
       <c r="J32" s="53" t="s">
         <v>26</v>
@@ -3878,13 +3980,13 @@
         <v>26</v>
       </c>
       <c r="N32" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O32" s="26" t="s">
         <v>35</v>
       </c>
       <c r="P32" s="26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Q32" s="29"/>
       <c r="R32" s="26"/>
@@ -3893,7 +3995,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="90">
+    <row r="33" spans="1:20" ht="409.5">
       <c r="A33" s="21">
         <v>91</v>
       </c>
@@ -3904,22 +4006,22 @@
         <v>23</v>
       </c>
       <c r="D33" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="E33" s="23" t="s">
         <v>89</v>
-      </c>
-      <c r="E33" s="23" t="s">
-        <v>90</v>
       </c>
       <c r="F33" s="24">
         <v>45211</v>
       </c>
       <c r="G33" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="H33" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="H33" s="25" t="s">
+      <c r="I33" s="26" t="s">
         <v>175</v>
-      </c>
-      <c r="I33" s="26" t="s">
-        <v>176</v>
       </c>
       <c r="J33" s="53" t="s">
         <v>26</v>
@@ -3932,13 +4034,13 @@
         <v>26</v>
       </c>
       <c r="N33" s="28" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="O33" s="26" t="s">
         <v>35</v>
       </c>
       <c r="P33" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q33" s="29"/>
       <c r="R33" s="26"/>
@@ -3947,7 +4049,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="180">
+    <row r="34" spans="1:20" ht="285">
       <c r="A34" s="21">
         <v>92</v>
       </c>
@@ -3958,22 +4060,22 @@
         <v>23</v>
       </c>
       <c r="D34" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="E34" s="23" t="s">
         <v>92</v>
-      </c>
-      <c r="E34" s="23" t="s">
-        <v>93</v>
       </c>
       <c r="F34" s="24">
         <v>45211</v>
       </c>
       <c r="G34" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="H34" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="H34" s="26" t="s">
+      <c r="I34" s="55" t="s">
         <v>178</v>
-      </c>
-      <c r="I34" s="55" t="s">
-        <v>179</v>
       </c>
       <c r="J34" s="53" t="s">
         <v>26</v>
@@ -3986,13 +4088,13 @@
         <v>26</v>
       </c>
       <c r="N34" s="28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="O34" s="26" t="s">
         <v>35</v>
       </c>
       <c r="P34" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Q34" s="29"/>
       <c r="R34" s="26"/>
@@ -4001,61 +4103,61 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:20" s="90" customFormat="1" ht="180">
-      <c r="A35" s="78">
+    <row r="35" spans="1:20" s="81" customFormat="1" ht="285.75" thickBot="1">
+      <c r="A35" s="69">
         <v>93</v>
       </c>
-      <c r="B35" s="79" t="s">
+      <c r="B35" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="C35" s="79" t="s">
+      <c r="C35" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="79" t="s">
+      <c r="D35" s="70" t="s">
+        <v>94</v>
+      </c>
+      <c r="E35" s="71" t="s">
         <v>95</v>
       </c>
-      <c r="E35" s="80" t="s">
-        <v>96</v>
-      </c>
-      <c r="F35" s="81">
+      <c r="F35" s="72">
         <v>45223</v>
       </c>
-      <c r="G35" s="82" t="s">
+      <c r="G35" s="73" t="s">
+        <v>183</v>
+      </c>
+      <c r="H35" s="74" t="s">
+        <v>182</v>
+      </c>
+      <c r="I35" s="82" t="s">
         <v>184</v>
       </c>
-      <c r="H35" s="83" t="s">
-        <v>183</v>
-      </c>
-      <c r="I35" s="91" t="s">
+      <c r="J35" s="75" t="s">
+        <v>26</v>
+      </c>
+      <c r="K35" s="76"/>
+      <c r="L35" s="74" t="s">
+        <v>26</v>
+      </c>
+      <c r="M35" s="74" t="s">
+        <v>26</v>
+      </c>
+      <c r="N35" s="77" t="s">
         <v>185</v>
       </c>
-      <c r="J35" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="K35" s="85"/>
-      <c r="L35" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="M35" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="N35" s="86" t="s">
+      <c r="O35" s="74" t="s">
+        <v>35</v>
+      </c>
+      <c r="P35" s="74" t="s">
         <v>186</v>
       </c>
-      <c r="O35" s="83" t="s">
-        <v>35</v>
-      </c>
-      <c r="P35" s="83" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q35" s="88"/>
-      <c r="R35" s="83"/>
-      <c r="S35" s="89"/>
-      <c r="T35" s="83" t="s">
+      <c r="Q35" s="79"/>
+      <c r="R35" s="74"/>
+      <c r="S35" s="80"/>
+      <c r="T35" s="74" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:20">
+    <row r="36" spans="1:20" ht="15.75" thickBot="1">
       <c r="A36" s="60"/>
       <c r="B36" s="60"/>
       <c r="C36" s="60"/>
@@ -4071,7 +4173,7 @@
       <c r="M36" s="64"/>
       <c r="N36" s="63"/>
       <c r="O36" s="64"/>
-      <c r="P36" s="63"/>
+      <c r="P36" s="92"/>
       <c r="Q36" s="63"/>
       <c r="R36" s="65"/>
       <c r="S36" s="66"/>
@@ -4093,7 +4195,7 @@
       <c r="M37" s="37"/>
       <c r="N37" s="36"/>
       <c r="O37" s="37"/>
-      <c r="P37" s="36"/>
+      <c r="P37" s="93"/>
       <c r="Q37" s="36"/>
       <c r="R37" s="38"/>
       <c r="S37" s="39"/>
@@ -22697,40 +22799,40 @@
         <v>3</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>97</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>98</v>
       </c>
       <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="11" t="s">
         <v>101</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>102</v>
       </c>
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="C3" s="14" t="s">
+      <c r="D3" s="15" t="s">
         <v>104</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>105</v>
       </c>
       <c r="E3" s="7"/>
     </row>
@@ -22739,58 +22841,58 @@
         <v>23</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C4" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="16" t="s">
         <v>106</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>107</v>
       </c>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" ht="14.25" customHeight="1">
       <c r="A5" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="C5" s="14" t="s">
+      <c r="D5" s="15" t="s">
         <v>109</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>110</v>
       </c>
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" customHeight="1">
       <c r="A6" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="C6" s="14" t="s">
+      <c r="D6" s="16" t="s">
         <v>112</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>113</v>
       </c>
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" ht="14.25" customHeight="1">
       <c r="A7" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" s="19" t="s">
+      <c r="D7" s="16" t="s">
         <v>115</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>116</v>
       </c>
       <c r="E7" s="7"/>
     </row>

</xml_diff>